<commit_message>
no sale el loop
</commit_message>
<xml_diff>
--- a/BI_CARGA_EXTERNO 07 01 22.xlsx
+++ b/BI_CARGA_EXTERNO 07 01 22.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilde\Desktop\Desarrollo Cambiaria\AppCambiaria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rserdan\Desktop\Desarrollo Cambiaria\AppCambiaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="-32676" windowWidth="16596" windowHeight="1176" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="-32670" windowWidth="16590" windowHeight="1170" tabRatio="599"/>
   </bookViews>
   <sheets>
     <sheet name="COMPROBANTES" sheetId="1" r:id="rId1"/>
@@ -40771,36 +40771,38 @@
   </sheetPr>
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="9" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="9" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="9" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="21" customWidth="1"/>
-    <col min="6" max="8" width="12.6640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="98.44140625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="17" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" style="11" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" style="11" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="37.109375" style="10" customWidth="1"/>
-    <col min="17" max="17" width="22.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="9" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="9" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="9" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="66.140625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="11" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="11" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="37.140625" style="10" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" style="10" customWidth="1"/>
-    <col min="19" max="19" width="14.44140625" style="10" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="10"/>
+    <col min="19" max="19" width="14.42578125" style="10" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -40851,7 +40853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>16</v>
       </c>
@@ -40905,7 +40907,7 @@
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
     </row>
-    <row r="3" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
@@ -40956,7 +40958,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>27</v>
       </c>
@@ -41007,7 +41009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>16</v>
       </c>
@@ -41058,7 +41060,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>16</v>
       </c>
@@ -41109,7 +41111,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>16</v>
       </c>
@@ -41160,7 +41162,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
@@ -41211,7 +41213,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>16</v>
       </c>
@@ -41262,7 +41264,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -41313,7 +41315,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>43</v>
       </c>
@@ -41364,7 +41366,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>27</v>
       </c>
@@ -41415,7 +41417,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>62</v>
       </c>
@@ -41466,7 +41468,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>27</v>
       </c>
@@ -41517,7 +41519,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
@@ -41568,7 +41570,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>43</v>
       </c>
@@ -41619,7 +41621,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>16</v>
       </c>
@@ -41670,7 +41672,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>16</v>
       </c>
@@ -41721,7 +41723,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>16</v>
       </c>
@@ -41772,7 +41774,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>16</v>
       </c>
@@ -41823,7 +41825,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>16</v>
       </c>
@@ -41874,7 +41876,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>16</v>
       </c>
@@ -41925,7 +41927,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
         <v>16</v>
       </c>
@@ -41976,7 +41978,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>16</v>
       </c>
@@ -42027,7 +42029,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>16</v>
       </c>
@@ -42078,7 +42080,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>16</v>
       </c>
@@ -42129,7 +42131,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>16</v>
       </c>
@@ -42183,7 +42185,7 @@
       <c r="R27" s="27"/>
       <c r="S27" s="27"/>
     </row>
-    <row r="28" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>16</v>
       </c>
@@ -42237,7 +42239,7 @@
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
     </row>
-    <row r="29" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>16</v>
       </c>
@@ -42288,7 +42290,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>16</v>
       </c>
@@ -42339,7 +42341,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>16</v>
       </c>
@@ -42393,7 +42395,7 @@
       <c r="R31" s="33"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>16</v>
       </c>
@@ -42444,7 +42446,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>16</v>
       </c>
@@ -42498,7 +42500,7 @@
       <c r="R33" s="33"/>
       <c r="S33" s="33"/>
     </row>
-    <row r="34" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
         <v>16</v>
       </c>
@@ -42552,7 +42554,7 @@
         <v>5959047.8600000003</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>16</v>
       </c>
@@ -42610,7 +42612,7 @@
         <v>948168.81000000052</v>
       </c>
     </row>
-    <row r="36" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>16</v>
       </c>
@@ -42664,7 +42666,7 @@
         <v>3547937.34</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>16</v>
       </c>
@@ -42722,7 +42724,7 @@
         <v>418039.79999999981</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>16</v>
       </c>
@@ -42773,7 +42775,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>16</v>
       </c>
@@ -42824,7 +42826,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>16</v>
       </c>
@@ -42875,7 +42877,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>16</v>
       </c>
@@ -42926,7 +42928,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>27</v>
       </c>
@@ -42977,7 +42979,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="43" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>16</v>
       </c>
@@ -43028,7 +43030,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>16</v>
       </c>
@@ -43079,7 +43081,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>132</v>
       </c>
@@ -43130,7 +43132,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>132</v>
       </c>
@@ -43181,7 +43183,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>132</v>
       </c>
@@ -43232,7 +43234,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>132</v>
       </c>
@@ -43286,19 +43288,19 @@
       <c r="R48" s="33"/>
       <c r="S48" s="33"/>
     </row>
-    <row r="53" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M53" s="17">
         <f>+SUM(M2:M32)</f>
         <v>51767591.860000007</v>
       </c>
     </row>
-    <row r="54" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M54" s="17">
         <f>+SUM(M33:M48)</f>
         <v>20188507.240000002</v>
       </c>
     </row>
-    <row r="55" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M55" s="17">
         <f>+M53-M54</f>
         <v>31579084.620000005</v>
@@ -43324,23 +43326,23 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="79" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="79" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="56.5546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="32.5546875" style="2"/>
+    <col min="1" max="1" width="18.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="56.5703125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="32.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>148</v>
       </c>
@@ -43366,7 +43368,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>148</v>
       </c>
@@ -43389,7 +43391,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>148</v>
       </c>
@@ -43415,7 +43417,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>148</v>
       </c>
@@ -43441,7 +43443,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>148</v>
       </c>
@@ -43467,7 +43469,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>148</v>
       </c>
@@ -43493,7 +43495,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>148</v>
       </c>
@@ -43516,7 +43518,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>148</v>
       </c>
@@ -43539,7 +43541,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>148</v>
       </c>
@@ -43562,7 +43564,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>148</v>
       </c>
@@ -43588,7 +43590,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>148</v>
       </c>
@@ -43614,7 +43616,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>148</v>
       </c>
@@ -43640,7 +43642,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>148</v>
       </c>
@@ -43663,7 +43665,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>148</v>
       </c>
@@ -43689,7 +43691,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>148</v>
       </c>
@@ -43715,7 +43717,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>148</v>
       </c>
@@ -43741,7 +43743,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>148</v>
       </c>
@@ -43764,7 +43766,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>148</v>
       </c>
@@ -43790,7 +43792,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>148</v>
       </c>
@@ -43813,7 +43815,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>148</v>
       </c>
@@ -43836,7 +43838,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>148</v>
       </c>
@@ -43862,7 +43864,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>148</v>
       </c>
@@ -43888,7 +43890,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>148</v>
       </c>
@@ -43914,7 +43916,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>148</v>
       </c>
@@ -43940,7 +43942,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>148</v>
       </c>
@@ -43966,7 +43968,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>148</v>
       </c>
@@ -43989,7 +43991,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>148</v>
       </c>
@@ -44012,7 +44014,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>148</v>
       </c>
@@ -44035,7 +44037,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>148</v>
       </c>
@@ -44061,7 +44063,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>148</v>
       </c>
@@ -44087,7 +44089,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>148</v>
       </c>
@@ -44113,7 +44115,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>148</v>
       </c>
@@ -44139,7 +44141,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>148</v>
       </c>
@@ -44162,7 +44164,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>148</v>
       </c>
@@ -44185,7 +44187,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>148</v>
       </c>
@@ -44208,7 +44210,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>148</v>
       </c>
@@ -44231,7 +44233,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
@@ -44257,7 +44259,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>148</v>
       </c>
@@ -44280,7 +44282,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>148</v>
       </c>
@@ -44306,7 +44308,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>148</v>
       </c>
@@ -44329,7 +44331,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>148</v>
       </c>
@@ -44355,7 +44357,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>148</v>
       </c>
@@ -44381,7 +44383,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>148</v>
       </c>
@@ -44404,7 +44406,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>148</v>
       </c>
@@ -44430,7 +44432,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>148</v>
       </c>
@@ -44456,7 +44458,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>148</v>
       </c>
@@ -44479,7 +44481,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>148</v>
       </c>
@@ -44505,7 +44507,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>148</v>
       </c>
@@ -44531,7 +44533,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>148</v>
       </c>
@@ -44557,7 +44559,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
@@ -44583,7 +44585,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>148</v>
       </c>
@@ -44609,7 +44611,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>148</v>
       </c>
@@ -44635,7 +44637,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>148</v>
       </c>
@@ -44658,7 +44660,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>148</v>
       </c>
@@ -44684,7 +44686,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>148</v>
       </c>
@@ -44707,7 +44709,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>148</v>
       </c>
@@ -44730,7 +44732,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>148</v>
       </c>
@@ -44756,7 +44758,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>148</v>
       </c>
@@ -44779,7 +44781,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>148</v>
       </c>
@@ -44802,7 +44804,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>148</v>
       </c>
@@ -44825,7 +44827,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>148</v>
       </c>
@@ -44848,7 +44850,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>148</v>
       </c>
@@ -44874,7 +44876,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>148</v>
       </c>
@@ -44900,7 +44902,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>148</v>
       </c>
@@ -44926,7 +44928,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>148</v>
       </c>
@@ -44949,7 +44951,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>148</v>
       </c>
@@ -44972,7 +44974,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>148</v>
       </c>
@@ -44995,7 +44997,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>148</v>
       </c>
@@ -45018,7 +45020,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>148</v>
       </c>
@@ -45044,7 +45046,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G70" s="8"/>
     </row>
   </sheetData>

</xml_diff>